<commit_message>
Created docs folder, added headings for science-questions and geography-questions
</commit_message>
<xml_diff>
--- a/material/geography/geography-questions.xlsx
+++ b/material/geography/geography-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekaanshmurthy/Documents/GitHub/beescholar.github.io/material/geography/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{704136A5-1E27-8546-AEF9-C8255C67511C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658B0243-650C-AF4E-9FBD-698B9D5E367C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16760" xr2:uid="{E9A39F92-BA39-3E44-AB92-113DF4C36278}"/>
   </bookViews>
@@ -30,6 +30,29 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>questionId</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>answers</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>subtopic</t>
+  </si>
+  <si>
+    <t>difficulty</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +402,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05844486-99C0-9C48-8555-4DDC7C0CA4AA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>